<commit_message>
Results and Analysis added to report, form data charts created
</commit_message>
<xml_diff>
--- a/Paperwork/Testing/Website 1 Form Data.xlsx
+++ b/Paperwork/Testing/Website 1 Form Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GreenJames(2015)\git\A_Study_In_HCI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GreenJames(2015)\git\A_Study_In_HCI\Paperwork\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="90">
   <si>
     <t>Overall how did the website look?</t>
   </si>
@@ -272,41 +272,38 @@
     <t>Both close but the green gradients were unusual</t>
   </si>
   <si>
-    <t>Variant</t>
-  </si>
-  <si>
-    <t>Avg Look</t>
-  </si>
-  <si>
-    <t>Avg Feel</t>
-  </si>
-  <si>
-    <t>Avg Formal</t>
-  </si>
-  <si>
-    <t>Avg Informal</t>
-  </si>
-  <si>
-    <t>Avg Relaxing</t>
-  </si>
-  <si>
-    <t>Preference</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Look</t>
+  </si>
+  <si>
+    <t>Feel</t>
+  </si>
+  <si>
+    <t>Prefer A</t>
+  </si>
+  <si>
+    <t>Prefer B</t>
+  </si>
+  <si>
+    <t># Formal</t>
+  </si>
+  <si>
+    <t># Informal</t>
+  </si>
+  <si>
+    <t># Relaxing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,11 +318,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -423,20 +425,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,6 +455,3112 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Website 1 Comparisons</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Look</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$35:$L$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$36:$L$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.3571428571428577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B133-4663-B753-45DDF2C98AE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Feel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$35:$L$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$37:$L$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.8571428571428577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6071428571428577</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B133-4663-B753-45DDF2C98AE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="436761384"/>
+        <c:axId val="436757776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="436761384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436757776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="436757776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436761384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Website 1 Overall Preference</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4ED4-4D8B-8F89-22D6D90BD4C0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-4ED4-4D8B-8F89-22D6D90BD4C0}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-4ED4-4D8B-8F89-22D6D90BD4C0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-4ED4-4D8B-8F89-22D6D90BD4C0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$F$31:$F$32</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Prefer A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Prefer B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$31:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4ED4-4D8B-8F89-22D6D90BD4C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Descriptive Words</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Formal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$41:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C156-4754-946E-2868911BE4DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Informal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$41:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C156-4754-946E-2868911BE4DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Relaxing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$41:$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$44:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C156-4754-946E-2868911BE4DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="525395256"/>
+        <c:axId val="525394600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="525395256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Variant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525394600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="525394600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>User</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Votes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525395256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BE4C50B-6D2B-4AAF-B253-0EACB820740D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1214437</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DF224DE-90DE-4C95-BC65-84715C10F1F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F4B1FB5-F2D3-4BDA-9CEA-2342ED408045}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -752,10 +3860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1FD6DA-0D12-466E-872F-F9705DE4C20A}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,129 +4737,96 @@
         <f t="shared" si="0"/>
         <v>8.6071428571428577</v>
       </c>
+      <c r="F31" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G31">
         <f>COUNTIF(G2:G29, "*Variant A*")</f>
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="G32">
         <f>COUNTIF(G2:G29, "*Variant B*")</f>
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="L35" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="4" t="s">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="K36">
+        <f>AVERAGE(A1:A29)</f>
+        <v>8.3571428571428577</v>
+      </c>
+      <c r="L36">
+        <f>AVERAGE(D1:D29)</f>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="4" t="s">
+      <c r="K37">
+        <f>AVERAGE(B1:B29)</f>
+        <v>8.8571428571428577</v>
+      </c>
+      <c r="L37">
+        <f>AVERAGE(E1:E29)</f>
+        <v>8.6071428571428577</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="B42" s="6">
+        <v>21</v>
+      </c>
+      <c r="C42" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="B43" s="7">
+        <v>2</v>
+      </c>
+      <c r="C43" s="7">
+        <v>18</v>
+      </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="7">
-        <v>8.4</v>
-      </c>
-      <c r="C36" s="7">
-        <v>8.9</v>
-      </c>
-      <c r="D36" s="6">
-        <v>21</v>
-      </c>
-      <c r="E36" s="6">
-        <v>2</v>
-      </c>
-      <c r="F36" s="6">
+      <c r="B44" s="7">
         <v>4</v>
       </c>
-      <c r="G36" s="6">
-        <v>16</v>
-      </c>
-      <c r="H36" s="6">
-        <f>SUM(B36:G36)</f>
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="6">
-        <v>7.8</v>
-      </c>
-      <c r="C37" s="6">
-        <v>8.6</v>
-      </c>
-      <c r="D37" s="6">
-        <v>2</v>
-      </c>
-      <c r="E37" s="6">
+      <c r="C44" s="7">
         <v>18</v>
-      </c>
-      <c r="F37" s="6">
-        <v>18</v>
-      </c>
-      <c r="G37" s="6">
-        <v>12</v>
-      </c>
-      <c r="H37" s="6">
-        <f>SUM(B37:G37)</f>
-        <v>66.400000000000006</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="6">
-        <f>SUM(B36:B37)</f>
-        <v>16.2</v>
-      </c>
-      <c r="C38" s="6">
-        <f t="shared" ref="C38:H38" si="1">SUM(C36:C37)</f>
-        <v>17.5</v>
-      </c>
-      <c r="D38" s="6">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="E38" s="6">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="F38" s="6">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="G38" s="6">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="H38" s="6">
-        <f t="shared" si="1"/>
-        <v>126.7</v>
       </c>
     </row>
   </sheetData>
@@ -1762,5 +4837,6 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>